<commit_message>
- Added experimentation sheet for DS1 - Added default output buffers for DS1
</commit_message>
<xml_diff>
--- a/Data set release 1/ds1/stats.xlsx
+++ b/Data set release 1/ds1/stats.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\soen472_mp2\Data set release 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\soen472_mp2\Data set release 1\ds1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7186A6A5-12BF-4928-A790-3FE11576CA03}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4595BCCB-DB67-4847-A499-313C021CBA08}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" activeTab="2" xr2:uid="{E3F65C83-32B3-4C7A-966E-A0762FD703F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
     <sheet name="Validation" sheetId="3" r:id="rId2"/>
-    <sheet name="Testing" sheetId="2" r:id="rId3"/>
+    <sheet name="Experimentation" sheetId="4" r:id="rId3"/>
+    <sheet name="Testing" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>Algorithm</t>
   </si>
@@ -65,6 +66,96 @@
   </si>
   <si>
     <t>Multilayer Perceptron (500 epochs / 51 hidden nodes)</t>
+  </si>
+  <si>
+    <t>Using same hyper-parameters as training</t>
+  </si>
+  <si>
+    <t>Effects</t>
+  </si>
+  <si>
+    <t>Do not check capabilities</t>
+  </si>
+  <si>
+    <t>Use kernel estimator</t>
+  </si>
+  <si>
+    <t>Use supervised discretization</t>
+  </si>
+  <si>
+    <t>Hyper-parameters</t>
+  </si>
+  <si>
+    <t>Binary splits</t>
+  </si>
+  <si>
+    <t>Collapse tree</t>
+  </si>
+  <si>
+    <t>Confidence factor</t>
+  </si>
+  <si>
+    <t>Do not make split point actual value</t>
+  </si>
+  <si>
+    <t>Min num obj</t>
+  </si>
+  <si>
+    <t>Num folds</t>
+  </si>
+  <si>
+    <t>Reduced error pruning</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Subtree raising</t>
+  </si>
+  <si>
+    <t>Unpruned</t>
+  </si>
+  <si>
+    <t>Use Laplace</t>
+  </si>
+  <si>
+    <t>Use MDL correction</t>
+  </si>
+  <si>
+    <t>Decay</t>
+  </si>
+  <si>
+    <t>Hidden layers</t>
+  </si>
+  <si>
+    <t>Learning rate</t>
+  </si>
+  <si>
+    <t>Momentum</t>
+  </si>
+  <si>
+    <t>Nominal to binary filter</t>
+  </si>
+  <si>
+    <t>Normalize attributes</t>
+  </si>
+  <si>
+    <t>Normalize numeric class</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Training time</t>
+  </si>
+  <si>
+    <t>Validation set size</t>
+  </si>
+  <si>
+    <t>Validation threshold</t>
+  </si>
+  <si>
+    <t>Note: DS1 is balanced</t>
   </si>
 </sst>
 </file>
@@ -72,9 +163,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,13 +181,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,20 +227,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -436,7 +563,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,19 +699,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E241F916-2D09-489E-8D95-B541D8A8FAFC}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" customWidth="1"/>
-    <col min="2" max="2" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="13.6328125" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -608,23 +733,69 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="C2">
+        <v>0.621</v>
+      </c>
+      <c r="D2">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="E2">
+        <v>0.59799999999999998</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="C3">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="D3">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="E3">
+        <v>0.33900000000000002</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>0.22</v>
+      </c>
+      <c r="C4">
+        <v>0.219</v>
+      </c>
+      <c r="D4">
+        <v>0.22</v>
+      </c>
+      <c r="E4">
+        <v>0.21099999999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B5">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="C5">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.56899999999999995</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
@@ -634,6 +805,208 @@
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="C7">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="D7">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="E7">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7A6426-F1A3-479C-A068-38DE87B162FB}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -641,11 +1014,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B99671A-CE46-469F-9F70-DE3054D56DC1}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>